<commit_message>
Added volume column. Ref #5
</commit_message>
<xml_diff>
--- a/data/source/proceedings_metadata.xlsx
+++ b/data/source/proceedings_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\andreas\data\proceedings\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\andreas\source\inidun\refactor\proceedings_curation\data\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6414AE5A-816C-40D9-A49F-0322A167727E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8CC1FB-73FF-4A1C-AEED-7C3A55F65758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32400" yWindow="2412" windowWidth="31068" windowHeight="18192" xr2:uid="{5A000467-A9F1-4111-9E70-7D0B8F2E230C}"/>
+    <workbookView xWindow="58770" yWindow="2280" windowWidth="31770" windowHeight="17115" xr2:uid="{5A000467-A9F1-4111-9E70-7D0B8F2E230C}"/>
   </bookViews>
   <sheets>
     <sheet name="proceedings_metadata.tsv" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="479">
   <si>
     <t>record_number</t>
   </si>
@@ -3291,6 +3291,9 @@
 a, m.
 President:
 Mr, Paulo E, de BERREDO CARNEIRO (Bruzil)</t>
+  </si>
+  <si>
+    <t>volume</t>
   </si>
 </sst>
 </file>
@@ -3342,7 +3345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3354,11 +3357,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -3436,41 +3443,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{496F955A-90C8-4603-BBDC-126471262674}" name="proceedings_metadata" displayName="proceedings_metadata" ref="A1:T44" totalsRowShown="0" headerRowDxfId="20">
-  <autoFilter ref="A1:T44" xr:uid="{496F955A-90C8-4603-BBDC-126471262674}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{496F955A-90C8-4603-BBDC-126471262674}" name="proceedings_metadata" displayName="proceedings_metadata" ref="A1:U44" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A1:U44" xr:uid="{496F955A-90C8-4603-BBDC-126471262674}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T44">
     <sortCondition ref="C1:C44"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{8813E9DE-138C-4A26-8F8A-468F8E1C25E8}" name="record_number" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{8A9D997C-DBB6-43D0-9B4E-2C8ABDB27553}" name="city" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{F6B88717-BAE0-4504-85E5-611A0647F79F}" name="year" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{CE087AC0-A261-4E24-9546-5AA33C3B338B}" name="filename" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{90F18FA6-4001-40E4-9324-805AEDC00E27}" name="has_text" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{1963AC70-ED02-48F7-958C-60C018FC115A}" name="extractable" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{4DB656F9-F564-4366-8C21-BB4BC2C2044B}" name="page_numbers" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{B600578E-743B-48E7-B9D7-AE1A2E309808}" name="pdf_page_numbers" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{60C7AD7D-70E3-4F2D-96CF-6D81A95F1973}" name="languages" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{88B1593B-9C55-42F0-A017-FB6A5D947C60}" name="born_digital" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{FB1AB437-5C66-44E1-A0CD-83235F1206BA}" name="primary_language" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{CD306B39-60FA-4FD5-929D-0A1221D5D2F0}" name="columns" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{305209BF-7778-4941-8163-31D855DB2AB1}" name="toc_pages" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{E0F3545E-4E57-4B58-BA11-C2EA2C3F1258}" name="header_session" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{20BDDCF3-D239-4794-8808-20FCC1D48A7F}" name="header_session_part" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{66E4BA30-3F29-4B38-AB23-B1F530FA5B43}" name="header_02" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{79AD2B5D-40AC-47F6-9A0E-33D31DE43F38}" name="start_of_speech" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{04F2C225-926A-4460-8CDC-650A3C6DC2B6}" name="start_of_paragraph" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{0F75E5EE-7510-45F5-A751-FF3C47185E44}" name="start_of_translation" dataDxfId="1"/>
-    <tableColumn id="20" xr3:uid="{A720F304-965C-429D-86D6-550191E1A925}" name="notes" dataDxfId="0"/>
+  <tableColumns count="21">
+    <tableColumn id="1" xr3:uid="{8813E9DE-138C-4A26-8F8A-468F8E1C25E8}" name="record_number" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{8A9D997C-DBB6-43D0-9B4E-2C8ABDB27553}" name="city" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{F6B88717-BAE0-4504-85E5-611A0647F79F}" name="year" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{CE087AC0-A261-4E24-9546-5AA33C3B338B}" name="filename" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{90F18FA6-4001-40E4-9324-805AEDC00E27}" name="has_text" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{1963AC70-ED02-48F7-958C-60C018FC115A}" name="extractable" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{4DB656F9-F564-4366-8C21-BB4BC2C2044B}" name="page_numbers" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{B600578E-743B-48E7-B9D7-AE1A2E309808}" name="pdf_page_numbers" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{60C7AD7D-70E3-4F2D-96CF-6D81A95F1973}" name="languages" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{88B1593B-9C55-42F0-A017-FB6A5D947C60}" name="born_digital" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{FB1AB437-5C66-44E1-A0CD-83235F1206BA}" name="primary_language" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{CD306B39-60FA-4FD5-929D-0A1221D5D2F0}" name="columns" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{305209BF-7778-4941-8163-31D855DB2AB1}" name="toc_pages" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{E0F3545E-4E57-4B58-BA11-C2EA2C3F1258}" name="header_session" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{20BDDCF3-D239-4794-8808-20FCC1D48A7F}" name="header_session_part" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{66E4BA30-3F29-4B38-AB23-B1F530FA5B43}" name="header_02" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{79AD2B5D-40AC-47F6-9A0E-33D31DE43F38}" name="start_of_speech" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{04F2C225-926A-4460-8CDC-650A3C6DC2B6}" name="start_of_paragraph" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{0F75E5EE-7510-45F5-A751-FF3C47185E44}" name="start_of_translation" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{A720F304-965C-429D-86D6-550191E1A925}" name="notes" dataDxfId="1"/>
+    <tableColumn id="21" xr3:uid="{B5FABFFE-0D7B-46DF-845B-D2F06A0A99B3}" name="volume" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3508,7 +3516,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3614,7 +3622,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3756,7 +3764,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3764,10 +3772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C97765-D135-45B5-843F-019667A50B5C}">
-  <dimension ref="A1:T44"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3793,7 +3801,7 @@
     <col min="20" max="20" width="46.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3854,8 +3862,11 @@
       <c r="T1" t="s">
         <v>15</v>
       </c>
+      <c r="U1" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" ht="185.25" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -3916,8 +3927,9 @@
       <c r="T2" t="s">
         <v>269</v>
       </c>
+      <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:20" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>200</v>
       </c>
@@ -3978,8 +3990,9 @@
       <c r="T3" t="s">
         <v>24</v>
       </c>
+      <c r="U3" s="5"/>
     </row>
-    <row r="4" spans="1:20" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>217</v>
       </c>
@@ -4040,8 +4053,9 @@
       <c r="T4" t="s">
         <v>269</v>
       </c>
+      <c r="U4" s="5"/>
     </row>
-    <row r="5" spans="1:20" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>193</v>
       </c>
@@ -4102,8 +4116,9 @@
       <c r="T5" t="s">
         <v>24</v>
       </c>
+      <c r="U5" s="5"/>
     </row>
-    <row r="6" spans="1:20" ht="114" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" ht="114" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>184</v>
       </c>
@@ -4164,8 +4179,9 @@
       <c r="T6" s="1" t="s">
         <v>270</v>
       </c>
+      <c r="U6" s="5"/>
     </row>
-    <row r="7" spans="1:20" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>176</v>
       </c>
@@ -4226,8 +4242,9 @@
       <c r="T7" t="s">
         <v>24</v>
       </c>
+      <c r="U7" s="5"/>
     </row>
-    <row r="8" spans="1:20" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" ht="213.75" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>208</v>
       </c>
@@ -4288,8 +4305,9 @@
       <c r="T8" s="1" t="s">
         <v>271</v>
       </c>
+      <c r="U8" s="5"/>
     </row>
-    <row r="9" spans="1:20" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -4350,8 +4368,9 @@
       <c r="T9" s="1" t="s">
         <v>471</v>
       </c>
+      <c r="U9" s="5"/>
     </row>
-    <row r="10" spans="1:20" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>148</v>
       </c>
@@ -4412,8 +4431,9 @@
       <c r="T10" s="1" t="s">
         <v>272</v>
       </c>
+      <c r="U10" s="5"/>
     </row>
-    <row r="11" spans="1:20" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>143</v>
       </c>
@@ -4474,8 +4494,9 @@
       <c r="T11" s="1" t="s">
         <v>273</v>
       </c>
+      <c r="U11" s="5"/>
     </row>
-    <row r="12" spans="1:20" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>139</v>
       </c>
@@ -4536,8 +4557,9 @@
       <c r="T12" s="1" t="s">
         <v>274</v>
       </c>
+      <c r="U12" s="5"/>
     </row>
-    <row r="13" spans="1:20" ht="171" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" ht="171" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -4598,8 +4620,9 @@
       <c r="T13" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="U13" s="5"/>
     </row>
-    <row r="14" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -4660,8 +4683,9 @@
       <c r="T14" s="1" t="s">
         <v>284</v>
       </c>
+      <c r="U14" s="5"/>
     </row>
-    <row r="15" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -4722,8 +4746,9 @@
       <c r="T15" t="s">
         <v>269</v>
       </c>
+      <c r="U15" s="5"/>
     </row>
-    <row r="16" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -4784,8 +4809,9 @@
       <c r="T16" s="1" t="s">
         <v>269</v>
       </c>
+      <c r="U16" s="5"/>
     </row>
-    <row r="17" spans="1:20" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" ht="313.5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>117</v>
       </c>
@@ -4846,8 +4872,9 @@
       <c r="T17" s="1" t="s">
         <v>305</v>
       </c>
+      <c r="U17" s="5"/>
     </row>
-    <row r="18" spans="1:20" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>155</v>
       </c>
@@ -4908,8 +4935,9 @@
       <c r="T18" s="1" t="s">
         <v>276</v>
       </c>
+      <c r="U18" s="5"/>
     </row>
-    <row r="19" spans="1:20" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" ht="356.25" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>167</v>
       </c>
@@ -4970,8 +4998,9 @@
       <c r="T19" t="s">
         <v>269</v>
       </c>
+      <c r="U19" s="5"/>
     </row>
-    <row r="20" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -5029,8 +5058,9 @@
       <c r="T20" t="s">
         <v>24</v>
       </c>
+      <c r="U20" s="5"/>
     </row>
-    <row r="21" spans="1:20" ht="342" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" ht="342" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -5091,8 +5121,9 @@
       <c r="T21" s="1" t="s">
         <v>277</v>
       </c>
+      <c r="U21" s="5"/>
     </row>
-    <row r="22" spans="1:20" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" ht="185.25" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -5153,8 +5184,11 @@
       <c r="T22" s="1" t="s">
         <v>278</v>
       </c>
+      <c r="U22" s="5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:20" ht="242.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" ht="242.25" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -5215,8 +5249,11 @@
       <c r="T23" s="1" t="s">
         <v>279</v>
       </c>
+      <c r="U23" s="5">
+        <v>2</v>
+      </c>
     </row>
-    <row r="24" spans="1:20" ht="370.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" ht="370.5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>213</v>
       </c>
@@ -5277,8 +5314,9 @@
       <c r="T24" t="s">
         <v>24</v>
       </c>
+      <c r="U24" s="5"/>
     </row>
-    <row r="25" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>226</v>
       </c>
@@ -5339,8 +5377,9 @@
       <c r="T25" t="s">
         <v>24</v>
       </c>
+      <c r="U25" s="5"/>
     </row>
-    <row r="26" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -5401,8 +5440,9 @@
       <c r="T26" s="1" t="s">
         <v>332</v>
       </c>
+      <c r="U26" s="5"/>
     </row>
-    <row r="27" spans="1:20" ht="399" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" ht="399" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -5460,8 +5500,9 @@
       <c r="T27" t="s">
         <v>341</v>
       </c>
+      <c r="U27" s="5"/>
     </row>
-    <row r="28" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -5522,8 +5563,9 @@
       <c r="T28" t="s">
         <v>24</v>
       </c>
+      <c r="U28" s="5"/>
     </row>
-    <row r="29" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -5581,8 +5623,9 @@
       <c r="S29" s="1" t="s">
         <v>348</v>
       </c>
+      <c r="U29" s="5"/>
     </row>
-    <row r="30" spans="1:20" ht="384.75" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21" ht="384.75" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -5643,8 +5686,9 @@
       <c r="T30" t="s">
         <v>341</v>
       </c>
+      <c r="U30" s="5"/>
     </row>
-    <row r="31" spans="1:20" ht="399" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21" ht="399" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -5705,8 +5749,9 @@
       <c r="T31" s="1" t="s">
         <v>332</v>
       </c>
+      <c r="U31" s="5"/>
     </row>
-    <row r="32" spans="1:20" ht="299.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:21" ht="299.25" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -5767,8 +5812,9 @@
       <c r="T32" t="s">
         <v>341</v>
       </c>
+      <c r="U32" s="5"/>
     </row>
-    <row r="33" spans="1:20" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:21" ht="356.25" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -5829,8 +5875,9 @@
       <c r="T33" t="s">
         <v>341</v>
       </c>
+      <c r="U33" s="5"/>
     </row>
-    <row r="34" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -5891,8 +5938,9 @@
       <c r="T34" t="s">
         <v>341</v>
       </c>
+      <c r="U34" s="5"/>
     </row>
-    <row r="35" spans="1:20" ht="370.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21" ht="370.5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -5953,8 +6001,9 @@
       <c r="T35" s="1" t="s">
         <v>374</v>
       </c>
+      <c r="U35" s="5"/>
     </row>
-    <row r="36" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>101</v>
       </c>
@@ -6015,8 +6064,9 @@
       <c r="T36" s="1" t="s">
         <v>380</v>
       </c>
+      <c r="U36" s="5"/>
     </row>
-    <row r="37" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>105</v>
       </c>
@@ -6077,8 +6127,9 @@
       <c r="T37" s="1" t="s">
         <v>380</v>
       </c>
+      <c r="U37" s="5"/>
     </row>
-    <row r="38" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>109</v>
       </c>
@@ -6139,8 +6190,9 @@
       <c r="T38" s="1" t="s">
         <v>386</v>
       </c>
+      <c r="U38" s="5"/>
     </row>
-    <row r="39" spans="1:20" ht="270.75" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:21" ht="270.75" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>113</v>
       </c>
@@ -6201,8 +6253,9 @@
       <c r="T39" s="1" t="s">
         <v>390</v>
       </c>
+      <c r="U39" s="5"/>
     </row>
-    <row r="40" spans="1:20" ht="299.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:21" ht="299.25" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>171</v>
       </c>
@@ -6263,8 +6316,9 @@
       <c r="T40" s="1" t="s">
         <v>395</v>
       </c>
+      <c r="U40" s="5"/>
     </row>
-    <row r="41" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>231</v>
       </c>
@@ -6325,8 +6379,9 @@
       <c r="T41" s="1" t="s">
         <v>401</v>
       </c>
+      <c r="U41" s="5"/>
     </row>
-    <row r="42" spans="1:20" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:21" ht="313.5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>222</v>
       </c>
@@ -6387,8 +6442,9 @@
       <c r="T42" s="1" t="s">
         <v>401</v>
       </c>
+      <c r="U42" s="5"/>
     </row>
-    <row r="43" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>235</v>
       </c>
@@ -6449,8 +6505,9 @@
       <c r="T43" s="1" t="s">
         <v>401</v>
       </c>
+      <c r="U43" s="5"/>
     </row>
-    <row r="44" spans="1:20" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>239</v>
       </c>
@@ -6511,6 +6568,7 @@
       <c r="T44" s="1" t="s">
         <v>401</v>
       </c>
+      <c r="U44" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>